<commit_message>
Revert "Use Keshia's updated xls"
This reverts commit 390a1dba8a9facdacc0b5dddd42cc9ef2b078547.
</commit_message>
<xml_diff>
--- a/Product Inventory.xlsx
+++ b/Product Inventory.xlsx
@@ -10,7 +10,8 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:vt="http://schemas.openxmlformats.org/officeDocument/2006/docPropsVTypes">
-  <numFmts count="1">
+  <numFmts count="2">
+    <numFmt numFmtId="6" formatCode="&quot;$&quot;#,##0_);[Red]\(&quot;$&quot;#,##0\)"/>
     <numFmt numFmtId="56" formatCode="&quot;上午/下午 &quot;hh&quot;時&quot;mm&quot;分&quot;ss&quot;秒 &quot;"/>
   </numFmts>
   <fonts count="1">
@@ -403,16 +404,16 @@
         <v>1</v>
       </c>
       <c r="B2" t="str">
-        <v>Pink Penguin Puppy Chow</v>
+        <v>Canon imageCLASS 2200 Advanced Copier</v>
       </c>
       <c r="C2">
         <v>51100</v>
       </c>
       <c r="D2">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="E2">
-        <v>12</v>
+        <v>2</v>
       </c>
     </row>
     <row r="3">
@@ -420,7 +421,7 @@
         <v>2</v>
       </c>
       <c r="B3" t="str">
-        <v>Corneli Calming Collar™</v>
+        <v>Fellowes PB500 Electric Punch Plastic Comb Binding Machine with Manual Bind</v>
       </c>
       <c r="C3">
         <v>25928</v>
@@ -437,7 +438,7 @@
         <v>3</v>
       </c>
       <c r="B4" t="str">
-        <v>YELLOW Homestyle® Adult Dog Food</v>
+        <v>Cisco TelePresence System EX90 Videoconferencing Unit</v>
       </c>
       <c r="C4">
         <v>22638</v>
@@ -454,7 +455,7 @@
         <v>4</v>
       </c>
       <c r="B5" t="str">
-        <v>Robinson's Best® Anti Chew Spray</v>
+        <v>HON 5400 Series Task Chairs for Big and Tall</v>
       </c>
       <c r="C5">
         <v>21871</v>
@@ -471,7 +472,7 @@
         <v>5</v>
       </c>
       <c r="B6" t="str">
-        <v>Doggy Breath Freshener</v>
+        <v>GBC DocuBind TL300 Electric Binding System</v>
       </c>
       <c r="C6">
         <v>19823</v>
@@ -488,7 +489,7 @@
         <v>6</v>
       </c>
       <c r="B7" t="str">
-        <v>Royal® Adult Devplatypus Food</v>
+        <v>GBC Ibimaster 500 Manual ProClick Binding System</v>
       </c>
       <c r="C7">
         <v>19025</v>
@@ -505,7 +506,7 @@
         <v>7</v>
       </c>
       <c r="B8" t="str">
-        <v>Anti Fungal Spray</v>
+        <v>HP Designjet T520 Inkjet Large Format Printer - 24" Color</v>
       </c>
       <c r="C8">
         <v>18375</v>
@@ -522,7 +523,7 @@
         <v>8</v>
       </c>
       <c r="B9" t="str">
-        <v>Caring for your Narwhale by Jenn Petti</v>
+        <v>GBC DocuBind P400 Electric Binding System</v>
       </c>
       <c r="C9">
         <v>17965</v>
@@ -539,7 +540,7 @@
         <v>9</v>
       </c>
       <c r="B10" t="str">
-        <v>Bird Cage</v>
+        <v>High Speed Automatic Electric Letter Opener</v>
       </c>
       <c r="C10">
         <v>17030</v>
@@ -556,7 +557,7 @@
         <v>10</v>
       </c>
       <c r="B11" t="str">
-        <v>Bird Cage Floor Dressing</v>
+        <v>Lexmark MX611dhe Monochrome Laser Printer</v>
       </c>
       <c r="C11">
         <v>16830</v>
@@ -573,7 +574,7 @@
         <v>11</v>
       </c>
       <c r="B12" t="str">
-        <v>Sasquatch Feeder</v>
+        <v>Hewlett Packard LaserJet 3310 Copier</v>
       </c>
       <c r="C12">
         <v>15960</v>
@@ -590,7 +591,7 @@
         <v>12</v>
       </c>
       <c r="B13" t="str">
-        <v>Parrot Safety Harness</v>
+        <v>Riverside Palais Royal Lawyers Bookcase, Royale Cherry Finish</v>
       </c>
       <c r="C13">
         <v>15611</v>
@@ -607,7 +608,7 @@
         <v>13</v>
       </c>
       <c r="B14" t="str">
-        <v>Kearney Cat Collar™</v>
+        <v>Martin Yale Chadless Opener Electric Letter Opener</v>
       </c>
       <c r="C14">
         <v>14991</v>
@@ -624,7 +625,7 @@
         <v>14</v>
       </c>
       <c r="B15" t="str">
-        <v>ChowChow® Chewy Treats</v>
+        <v>3D Systems Cube Printer, 2nd Generation, Magenta</v>
       </c>
       <c r="C15">
         <v>14300</v>
@@ -641,7 +642,7 @@
         <v>15</v>
       </c>
       <c r="B16" t="str">
-        <v>Emo Chow</v>
+        <v>Ibico EPK-21 Electric Binding System</v>
       </c>
       <c r="C16">
         <v>13986</v>
@@ -658,7 +659,7 @@
         <v>16</v>
       </c>
       <c r="B17" t="str">
-        <v>AniMarty® Fish Flakes</v>
+        <v>Apple iPhone 5</v>
       </c>
       <c r="C17">
         <v>12997</v>
@@ -675,7 +676,7 @@
         <v>17</v>
       </c>
       <c r="B18" t="str">
-        <v>Adult Dog Taco Costume</v>
+        <v>Bretford Rectangular Conference Table Tops</v>
       </c>
       <c r="C18">
         <v>12469</v>
@@ -692,7 +693,7 @@
         <v>18</v>
       </c>
       <c r="B19" t="str">
-        <v>Barker's Anti Bark Spray™</v>
+        <v>Samsung Galaxy Mega 6.3</v>
       </c>
       <c r="C19">
         <v>12012</v>
@@ -709,7 +710,7 @@
         <v>19</v>
       </c>
       <c r="B20" t="str">
-        <v>Rose® Collapsible Bowl</v>
+        <v>Canon PC1060 Personal Laser Copier</v>
       </c>
       <c r="C20">
         <v>11620</v>
@@ -726,7 +727,7 @@
         <v>20</v>
       </c>
       <c r="B21" t="str">
-        <v>Sasquatch Feed</v>
+        <v>Honeywell Enviracaire Portable HEPA Air Cleaner for 17' x 22' Room</v>
       </c>
       <c r="C21">
         <v>11304</v>
@@ -743,7 +744,7 @@
         <v>21</v>
       </c>
       <c r="B22" t="str">
-        <v>Lizard Coat</v>
+        <v>Cubify CubeX 3D Printer Double Head Print</v>
       </c>
       <c r="C22">
         <v>11100</v>
@@ -760,7 +761,7 @@
         <v>22</v>
       </c>
       <c r="B23" t="str">
-        <v>Ferret Vitamins</v>
+        <v>DMI Eclipse Executive Suite Bookcases</v>
       </c>
       <c r="C23">
         <v>11047</v>
@@ -777,7 +778,7 @@
         <v>23</v>
       </c>
       <c r="B24" t="str">
-        <v>Car Seat Covers</v>
+        <v>Tennsco 6- and 18-Compartment Lockers</v>
       </c>
       <c r="C24">
         <v>10925</v>
@@ -794,7 +795,7 @@
         <v>24</v>
       </c>
       <c r="B25" t="str">
-        <v>Adult Dog T-Rex Costume</v>
+        <v>Plantronics CS510 - Over-the-Head monaural Wireless Headset System</v>
       </c>
       <c r="C25">
         <v>10822</v>
@@ -811,7 +812,7 @@
         <v>25</v>
       </c>
       <c r="B26" t="str">
-        <v>Fox Car Safety Harness</v>
+        <v>Global Troy Executive Leather Low-Back Tilter</v>
       </c>
       <c r="C26">
         <v>10571</v>
@@ -828,7 +829,7 @@
         <v>26</v>
       </c>
       <c r="B27" t="str">
-        <v>Dog Agility Tunnel</v>
+        <v>Logitech P710e Mobile Speakerphone</v>
       </c>
       <c r="C27">
         <v>10197</v>
@@ -845,7 +846,7 @@
         <v>27</v>
       </c>
       <c r="B28" t="str">
-        <v>Fishpoo® Fish Shampoo</v>
+        <v>Chromcraft Bull-Nose Wood Oval Conference Tables &amp; Bases</v>
       </c>
       <c r="C28">
         <v>9918</v>
@@ -862,7 +863,7 @@
         <v>28</v>
       </c>
       <c r="B29" t="str">
-        <v>Carrot Plushie</v>
+        <v>SAFCO Arco Folding Chair</v>
       </c>
       <c r="C29">
         <v>9501</v>
@@ -879,7 +880,7 @@
         <v>29</v>
       </c>
       <c r="B30" t="str">
-        <v>Yeti Vitamins</v>
+        <v>Plantronics Savi W720 Multi-Device Wireless Headset System</v>
       </c>
       <c r="C30">
         <v>9367</v>
@@ -896,7 +897,7 @@
         <v>30</v>
       </c>
       <c r="B31" t="str">
-        <v>Freeze-Dried Beef Treats</v>
+        <v>Hon Deluxe Fabric Upholstered Stacking Chairs, Rounded Back</v>
       </c>
       <c r="C31">
         <v>9271</v>
@@ -913,7 +914,7 @@
         <v>31</v>
       </c>
       <c r="B32" t="str">
-        <v>Eton Mess® Dog Hoodie</v>
+        <v>Global Deluxe High-Back Manager's Chair</v>
       </c>
       <c r="C32">
         <v>8665</v>
@@ -930,7 +931,7 @@
         <v>32</v>
       </c>
       <c r="B33" t="str">
-        <v>Rudolph Antler Chews™</v>
+        <v>GuestStacker Chair with Chrome Finish Legs</v>
       </c>
       <c r="C33">
         <v>8550</v>
@@ -947,7 +948,7 @@
         <v>33</v>
       </c>
       <c r="B34" t="str">
-        <v>Snake Oil</v>
+        <v>Hon 4070 Series Pagoda Armless Upholstered Stacking Chairs</v>
       </c>
       <c r="C34">
         <v>8431</v>
@@ -964,7 +965,7 @@
         <v>34</v>
       </c>
       <c r="B35" t="str">
-        <v>Round Fish Bowl</v>
+        <v>Tennsco Double-Tier Lockers</v>
       </c>
       <c r="C35">
         <v>8371</v>
@@ -981,7 +982,7 @@
         <v>35</v>
       </c>
       <c r="B36" t="str">
-        <v>Parrot Nail Clippers</v>
+        <v>Hot File 7-Pocket, Floor Stand</v>
       </c>
       <c r="C36">
         <v>8138</v>
@@ -998,7 +999,7 @@
         <v>36</v>
       </c>
       <c r="B37" t="str">
-        <v>Kangaroo® Food Pouch</v>
+        <v>Tennsco Single-Tier Lockers</v>
       </c>
       <c r="C37">
         <v>8032</v>
@@ -1015,7 +1016,7 @@
         <v>37</v>
       </c>
       <c r="B38" t="str">
-        <v>Lice &amp; Mite Destroyer</v>
+        <v>Wilson Electronics DB Pro Signal Booster</v>
       </c>
       <c r="C38">
         <v>8019</v>
@@ -1032,7 +1033,7 @@
         <v>38</v>
       </c>
       <c r="B39" t="str">
-        <v>Fox Toothpaste</v>
+        <v>Hewlett Packard 610 Color Digital Copier / Printer</v>
       </c>
       <c r="C39">
         <v>8000</v>
@@ -1049,7 +1050,7 @@
         <v>39</v>
       </c>
       <c r="B40" t="str">
-        <v>Crunchy Dog Treats</v>
+        <v>Okidata MB760 Printer</v>
       </c>
       <c r="C40">
         <v>7834</v>
@@ -1066,7 +1067,7 @@
         <v>40</v>
       </c>
       <c r="B41" t="str">
-        <v>Mini Adult Dog Food</v>
+        <v>Bush Advantage Collection Racetrack Conference Table</v>
       </c>
       <c r="C41">
         <v>7763</v>
@@ -1083,7 +1084,7 @@
         <v>41</v>
       </c>
       <c r="B42" t="str">
-        <v>All-Purpose Pet Conditioner</v>
+        <v>Ativa V4110MDD Micro-Cut Shredder</v>
       </c>
       <c r="C42">
         <v>7700</v>
@@ -1100,7 +1101,7 @@
         <v>42</v>
       </c>
       <c r="B43" t="str">
-        <v>Dental Doggie Treat</v>
+        <v>Hon 4700 Series Mobuis Mid-Back Task Chairs with Adjustable Arms</v>
       </c>
       <c r="C43">
         <v>7582</v>
@@ -1117,7 +1118,7 @@
         <v>43</v>
       </c>
       <c r="B44" t="str">
-        <v>Puppy Snacks</v>
+        <v>Global Commerce Series High-Back Swivel/Tilt Chairs</v>
       </c>
       <c r="C44">
         <v>7580</v>
@@ -1134,7 +1135,7 @@
         <v>44</v>
       </c>
       <c r="B45" t="str">
-        <v>Dewormer</v>
+        <v>Canon Imageclass D680 Copier / Fax</v>
       </c>
       <c r="C45">
         <v>7560</v>

</xml_diff>

<commit_message>
Use Keshia's updated xls
</commit_message>
<xml_diff>
--- a/Product Inventory.xlsx
+++ b/Product Inventory.xlsx
@@ -10,8 +10,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:vt="http://schemas.openxmlformats.org/officeDocument/2006/docPropsVTypes">
-  <numFmts count="2">
-    <numFmt numFmtId="6" formatCode="&quot;$&quot;#,##0_);[Red]\(&quot;$&quot;#,##0\)"/>
+  <numFmts count="1">
     <numFmt numFmtId="56" formatCode="&quot;上午/下午 &quot;hh&quot;時&quot;mm&quot;分&quot;ss&quot;秒 &quot;"/>
   </numFmts>
   <fonts count="1">
@@ -404,16 +403,16 @@
         <v>1</v>
       </c>
       <c r="B2" t="str">
-        <v>Canon imageCLASS 2200 Advanced Copier</v>
+        <v>Pink Penguin Puppy Chow</v>
       </c>
       <c r="C2">
         <v>51100</v>
       </c>
       <c r="D2">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="E2">
-        <v>2</v>
+        <v>12</v>
       </c>
     </row>
     <row r="3">
@@ -421,7 +420,7 @@
         <v>2</v>
       </c>
       <c r="B3" t="str">
-        <v>Fellowes PB500 Electric Punch Plastic Comb Binding Machine with Manual Bind</v>
+        <v>Corneli Calming Collar™</v>
       </c>
       <c r="C3">
         <v>25928</v>
@@ -438,7 +437,7 @@
         <v>3</v>
       </c>
       <c r="B4" t="str">
-        <v>Cisco TelePresence System EX90 Videoconferencing Unit</v>
+        <v>YELLOW Homestyle® Adult Dog Food</v>
       </c>
       <c r="C4">
         <v>22638</v>
@@ -455,7 +454,7 @@
         <v>4</v>
       </c>
       <c r="B5" t="str">
-        <v>HON 5400 Series Task Chairs for Big and Tall</v>
+        <v>Robinson's Best® Anti Chew Spray</v>
       </c>
       <c r="C5">
         <v>21871</v>
@@ -472,7 +471,7 @@
         <v>5</v>
       </c>
       <c r="B6" t="str">
-        <v>GBC DocuBind TL300 Electric Binding System</v>
+        <v>Doggy Breath Freshener</v>
       </c>
       <c r="C6">
         <v>19823</v>
@@ -489,7 +488,7 @@
         <v>6</v>
       </c>
       <c r="B7" t="str">
-        <v>GBC Ibimaster 500 Manual ProClick Binding System</v>
+        <v>Royal® Adult Devplatypus Food</v>
       </c>
       <c r="C7">
         <v>19025</v>
@@ -506,7 +505,7 @@
         <v>7</v>
       </c>
       <c r="B8" t="str">
-        <v>HP Designjet T520 Inkjet Large Format Printer - 24" Color</v>
+        <v>Anti Fungal Spray</v>
       </c>
       <c r="C8">
         <v>18375</v>
@@ -523,7 +522,7 @@
         <v>8</v>
       </c>
       <c r="B9" t="str">
-        <v>GBC DocuBind P400 Electric Binding System</v>
+        <v>Caring for your Narwhale by Jenn Petti</v>
       </c>
       <c r="C9">
         <v>17965</v>
@@ -540,7 +539,7 @@
         <v>9</v>
       </c>
       <c r="B10" t="str">
-        <v>High Speed Automatic Electric Letter Opener</v>
+        <v>Bird Cage</v>
       </c>
       <c r="C10">
         <v>17030</v>
@@ -557,7 +556,7 @@
         <v>10</v>
       </c>
       <c r="B11" t="str">
-        <v>Lexmark MX611dhe Monochrome Laser Printer</v>
+        <v>Bird Cage Floor Dressing</v>
       </c>
       <c r="C11">
         <v>16830</v>
@@ -574,7 +573,7 @@
         <v>11</v>
       </c>
       <c r="B12" t="str">
-        <v>Hewlett Packard LaserJet 3310 Copier</v>
+        <v>Sasquatch Feeder</v>
       </c>
       <c r="C12">
         <v>15960</v>
@@ -591,7 +590,7 @@
         <v>12</v>
       </c>
       <c r="B13" t="str">
-        <v>Riverside Palais Royal Lawyers Bookcase, Royale Cherry Finish</v>
+        <v>Parrot Safety Harness</v>
       </c>
       <c r="C13">
         <v>15611</v>
@@ -608,7 +607,7 @@
         <v>13</v>
       </c>
       <c r="B14" t="str">
-        <v>Martin Yale Chadless Opener Electric Letter Opener</v>
+        <v>Kearney Cat Collar™</v>
       </c>
       <c r="C14">
         <v>14991</v>
@@ -625,7 +624,7 @@
         <v>14</v>
       </c>
       <c r="B15" t="str">
-        <v>3D Systems Cube Printer, 2nd Generation, Magenta</v>
+        <v>ChowChow® Chewy Treats</v>
       </c>
       <c r="C15">
         <v>14300</v>
@@ -642,7 +641,7 @@
         <v>15</v>
       </c>
       <c r="B16" t="str">
-        <v>Ibico EPK-21 Electric Binding System</v>
+        <v>Emo Chow</v>
       </c>
       <c r="C16">
         <v>13986</v>
@@ -659,7 +658,7 @@
         <v>16</v>
       </c>
       <c r="B17" t="str">
-        <v>Apple iPhone 5</v>
+        <v>AniMarty® Fish Flakes</v>
       </c>
       <c r="C17">
         <v>12997</v>
@@ -676,7 +675,7 @@
         <v>17</v>
       </c>
       <c r="B18" t="str">
-        <v>Bretford Rectangular Conference Table Tops</v>
+        <v>Adult Dog Taco Costume</v>
       </c>
       <c r="C18">
         <v>12469</v>
@@ -693,7 +692,7 @@
         <v>18</v>
       </c>
       <c r="B19" t="str">
-        <v>Samsung Galaxy Mega 6.3</v>
+        <v>Barker's Anti Bark Spray™</v>
       </c>
       <c r="C19">
         <v>12012</v>
@@ -710,7 +709,7 @@
         <v>19</v>
       </c>
       <c r="B20" t="str">
-        <v>Canon PC1060 Personal Laser Copier</v>
+        <v>Rose® Collapsible Bowl</v>
       </c>
       <c r="C20">
         <v>11620</v>
@@ -727,7 +726,7 @@
         <v>20</v>
       </c>
       <c r="B21" t="str">
-        <v>Honeywell Enviracaire Portable HEPA Air Cleaner for 17' x 22' Room</v>
+        <v>Sasquatch Feed</v>
       </c>
       <c r="C21">
         <v>11304</v>
@@ -744,7 +743,7 @@
         <v>21</v>
       </c>
       <c r="B22" t="str">
-        <v>Cubify CubeX 3D Printer Double Head Print</v>
+        <v>Lizard Coat</v>
       </c>
       <c r="C22">
         <v>11100</v>
@@ -761,7 +760,7 @@
         <v>22</v>
       </c>
       <c r="B23" t="str">
-        <v>DMI Eclipse Executive Suite Bookcases</v>
+        <v>Ferret Vitamins</v>
       </c>
       <c r="C23">
         <v>11047</v>
@@ -778,7 +777,7 @@
         <v>23</v>
       </c>
       <c r="B24" t="str">
-        <v>Tennsco 6- and 18-Compartment Lockers</v>
+        <v>Car Seat Covers</v>
       </c>
       <c r="C24">
         <v>10925</v>
@@ -795,7 +794,7 @@
         <v>24</v>
       </c>
       <c r="B25" t="str">
-        <v>Plantronics CS510 - Over-the-Head monaural Wireless Headset System</v>
+        <v>Adult Dog T-Rex Costume</v>
       </c>
       <c r="C25">
         <v>10822</v>
@@ -812,7 +811,7 @@
         <v>25</v>
       </c>
       <c r="B26" t="str">
-        <v>Global Troy Executive Leather Low-Back Tilter</v>
+        <v>Fox Car Safety Harness</v>
       </c>
       <c r="C26">
         <v>10571</v>
@@ -829,7 +828,7 @@
         <v>26</v>
       </c>
       <c r="B27" t="str">
-        <v>Logitech P710e Mobile Speakerphone</v>
+        <v>Dog Agility Tunnel</v>
       </c>
       <c r="C27">
         <v>10197</v>
@@ -846,7 +845,7 @@
         <v>27</v>
       </c>
       <c r="B28" t="str">
-        <v>Chromcraft Bull-Nose Wood Oval Conference Tables &amp; Bases</v>
+        <v>Fishpoo® Fish Shampoo</v>
       </c>
       <c r="C28">
         <v>9918</v>
@@ -863,7 +862,7 @@
         <v>28</v>
       </c>
       <c r="B29" t="str">
-        <v>SAFCO Arco Folding Chair</v>
+        <v>Carrot Plushie</v>
       </c>
       <c r="C29">
         <v>9501</v>
@@ -880,7 +879,7 @@
         <v>29</v>
       </c>
       <c r="B30" t="str">
-        <v>Plantronics Savi W720 Multi-Device Wireless Headset System</v>
+        <v>Yeti Vitamins</v>
       </c>
       <c r="C30">
         <v>9367</v>
@@ -897,7 +896,7 @@
         <v>30</v>
       </c>
       <c r="B31" t="str">
-        <v>Hon Deluxe Fabric Upholstered Stacking Chairs, Rounded Back</v>
+        <v>Freeze-Dried Beef Treats</v>
       </c>
       <c r="C31">
         <v>9271</v>
@@ -914,7 +913,7 @@
         <v>31</v>
       </c>
       <c r="B32" t="str">
-        <v>Global Deluxe High-Back Manager's Chair</v>
+        <v>Eton Mess® Dog Hoodie</v>
       </c>
       <c r="C32">
         <v>8665</v>
@@ -931,7 +930,7 @@
         <v>32</v>
       </c>
       <c r="B33" t="str">
-        <v>GuestStacker Chair with Chrome Finish Legs</v>
+        <v>Rudolph Antler Chews™</v>
       </c>
       <c r="C33">
         <v>8550</v>
@@ -948,7 +947,7 @@
         <v>33</v>
       </c>
       <c r="B34" t="str">
-        <v>Hon 4070 Series Pagoda Armless Upholstered Stacking Chairs</v>
+        <v>Snake Oil</v>
       </c>
       <c r="C34">
         <v>8431</v>
@@ -965,7 +964,7 @@
         <v>34</v>
       </c>
       <c r="B35" t="str">
-        <v>Tennsco Double-Tier Lockers</v>
+        <v>Round Fish Bowl</v>
       </c>
       <c r="C35">
         <v>8371</v>
@@ -982,7 +981,7 @@
         <v>35</v>
       </c>
       <c r="B36" t="str">
-        <v>Hot File 7-Pocket, Floor Stand</v>
+        <v>Parrot Nail Clippers</v>
       </c>
       <c r="C36">
         <v>8138</v>
@@ -999,7 +998,7 @@
         <v>36</v>
       </c>
       <c r="B37" t="str">
-        <v>Tennsco Single-Tier Lockers</v>
+        <v>Kangaroo® Food Pouch</v>
       </c>
       <c r="C37">
         <v>8032</v>
@@ -1016,7 +1015,7 @@
         <v>37</v>
       </c>
       <c r="B38" t="str">
-        <v>Wilson Electronics DB Pro Signal Booster</v>
+        <v>Lice &amp; Mite Destroyer</v>
       </c>
       <c r="C38">
         <v>8019</v>
@@ -1033,7 +1032,7 @@
         <v>38</v>
       </c>
       <c r="B39" t="str">
-        <v>Hewlett Packard 610 Color Digital Copier / Printer</v>
+        <v>Fox Toothpaste</v>
       </c>
       <c r="C39">
         <v>8000</v>
@@ -1050,7 +1049,7 @@
         <v>39</v>
       </c>
       <c r="B40" t="str">
-        <v>Okidata MB760 Printer</v>
+        <v>Crunchy Dog Treats</v>
       </c>
       <c r="C40">
         <v>7834</v>
@@ -1067,7 +1066,7 @@
         <v>40</v>
       </c>
       <c r="B41" t="str">
-        <v>Bush Advantage Collection Racetrack Conference Table</v>
+        <v>Mini Adult Dog Food</v>
       </c>
       <c r="C41">
         <v>7763</v>
@@ -1084,7 +1083,7 @@
         <v>41</v>
       </c>
       <c r="B42" t="str">
-        <v>Ativa V4110MDD Micro-Cut Shredder</v>
+        <v>All-Purpose Pet Conditioner</v>
       </c>
       <c r="C42">
         <v>7700</v>
@@ -1101,7 +1100,7 @@
         <v>42</v>
       </c>
       <c r="B43" t="str">
-        <v>Hon 4700 Series Mobuis Mid-Back Task Chairs with Adjustable Arms</v>
+        <v>Dental Doggie Treat</v>
       </c>
       <c r="C43">
         <v>7582</v>
@@ -1118,7 +1117,7 @@
         <v>43</v>
       </c>
       <c r="B44" t="str">
-        <v>Global Commerce Series High-Back Swivel/Tilt Chairs</v>
+        <v>Puppy Snacks</v>
       </c>
       <c r="C44">
         <v>7580</v>
@@ -1135,7 +1134,7 @@
         <v>44</v>
       </c>
       <c r="B45" t="str">
-        <v>Canon Imageclass D680 Copier / Fax</v>
+        <v>Dewormer</v>
       </c>
       <c r="C45">
         <v>7560</v>

</xml_diff>